<commit_message>
Made the following changes based on Eng. Mohamed Ali's requests: - Added SIQ as an excel sheet - Updated project plan and schedule
Signed-off-by: cipher_93 <mahmoud.hamdy.hassan93@gmail.com>
</commit_message>
<xml_diff>
--- a/Deliveries/Project Plan.xlsx
+++ b/Deliveries/Project Plan.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Schedule" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Project Plan</t>
   </si>
@@ -40,15 +40,9 @@
     <t>Deadline</t>
   </si>
   <si>
-    <t>Estimated Duration</t>
-  </si>
-  <si>
     <t>Description &amp; Comments</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Schedule</t>
   </si>
   <si>
@@ -100,7 +94,22 @@
     <t>Prepare CYRS</t>
   </si>
   <si>
-    <t>1 Day</t>
+    <t>Complete CYRS</t>
+  </si>
+  <si>
+    <t>Complete HIS</t>
+  </si>
+  <si>
+    <t>Complete SRS</t>
+  </si>
+  <si>
+    <t>Complete project plan and SIQ based on data from CYRS</t>
+  </si>
+  <si>
+    <t>Estimated Duration (Days)</t>
+  </si>
+  <si>
+    <t>Currently working on modifications asked by Eng. Mohamed Ali</t>
   </si>
 </sst>
 </file>
@@ -158,9 +167,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -169,13 +175,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
+  <dxfs count="17">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -215,32 +249,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:G20" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A4:G20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:G10" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A4:G10"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Member Name" dataDxfId="6"/>
-    <tableColumn id="2" name="Task Name" dataDxfId="5"/>
-    <tableColumn id="3" name="Task Type" dataDxfId="4"/>
-    <tableColumn id="4" name="Start Date" dataDxfId="3"/>
-    <tableColumn id="5" name="Deadline" dataDxfId="2"/>
-    <tableColumn id="6" name="Estimated Duration" dataDxfId="1"/>
-    <tableColumn id="7" name="Description &amp; Comments" dataDxfId="0"/>
+    <tableColumn id="1" name="Member Name" dataDxfId="14"/>
+    <tableColumn id="2" name="Task Name" dataDxfId="13"/>
+    <tableColumn id="3" name="Task Type" dataDxfId="12"/>
+    <tableColumn id="4" name="Start Date" dataDxfId="11"/>
+    <tableColumn id="5" name="Deadline" dataDxfId="10"/>
+    <tableColumn id="6" name="Estimated Duration (Days)" dataDxfId="0">
+      <calculatedColumnFormula>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Description &amp; Comments" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:G5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A4:G5"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Milestone"/>
-    <tableColumn id="2" name="Planned Start Date"/>
-    <tableColumn id="3" name="Actual Start Date"/>
-    <tableColumn id="4" name="Planned End Date"/>
-    <tableColumn id="5" name="Actual End Date"/>
-    <tableColumn id="6" name="Description &amp; Comments"/>
-    <tableColumn id="7" name="Column1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:F8" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A4:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Milestone" dataDxfId="8"/>
+    <tableColumn id="2" name="Planned Start Date" dataDxfId="7"/>
+    <tableColumn id="3" name="Actual Start Date" dataDxfId="6"/>
+    <tableColumn id="4" name="Planned End Date" dataDxfId="5"/>
+    <tableColumn id="5" name="Actual End Date" dataDxfId="4"/>
+    <tableColumn id="6" name="Description &amp; Comments" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -509,16 +544,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="23.3984375" customWidth="1"/>
     <col min="3" max="3" width="16.796875" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
     <col min="5" max="5" width="10.59765625" customWidth="1"/>
@@ -528,15 +563,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -546,13 +581,13 @@
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -562,13 +597,13 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -577,244 +612,160 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43853</v>
+      </c>
+      <c r="E5" s="4">
+        <v>43860</v>
+      </c>
+      <c r="F5" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43852</v>
+      </c>
+      <c r="E6" s="4">
+        <v>43858</v>
+      </c>
+      <c r="F6" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4">
+        <v>43852</v>
+      </c>
+      <c r="E7" s="4">
+        <v>43858</v>
+      </c>
+      <c r="F7" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43852</v>
+      </c>
+      <c r="E8" s="4">
+        <v>43858</v>
+      </c>
+      <c r="F8" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4">
+        <v>43852</v>
+      </c>
+      <c r="E9" s="4">
+        <v>43858</v>
+      </c>
+      <c r="F9" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="5">
-        <v>43853</v>
-      </c>
-      <c r="E5" s="5">
-        <v>43854</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="5">
-        <v>43852</v>
-      </c>
-      <c r="E6" s="5">
-        <v>43853</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="5">
-        <v>43852</v>
-      </c>
-      <c r="E7" s="5">
-        <v>43853</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="5">
-        <v>43852</v>
-      </c>
-      <c r="E8" s="5">
-        <v>43853</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="5">
-        <v>43852</v>
-      </c>
-      <c r="E9" s="5">
-        <v>43853</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="5">
-        <v>43852</v>
-      </c>
-      <c r="E10" s="5">
-        <v>43853</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="D10" s="4">
+        <v>43852</v>
+      </c>
+      <c r="E10" s="4">
+        <v>43858</v>
+      </c>
+      <c r="F10" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="G10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -830,10 +781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -843,13 +794,13 @@
     <col min="3" max="3" width="16.09765625" customWidth="1"/>
     <col min="4" max="4" width="17.19921875" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="22.296875" customWidth="1"/>
+    <col min="6" max="6" width="37.796875" customWidth="1"/>
     <col min="7" max="7" width="9.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -880,26 +831,95 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4">
+        <v>43852</v>
+      </c>
+      <c r="C5" s="4">
+        <v>43852</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43853</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4">
+        <v>43852</v>
+      </c>
+      <c r="C6" s="4">
+        <v>43852</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43853</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4">
+        <v>43852</v>
+      </c>
+      <c r="C7" s="4">
+        <v>43852</v>
+      </c>
+      <c r="D7" s="4">
+        <v>43853</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4">
+        <v>43853</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43852</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43854</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert " "CYRS Updating""
</commit_message>
<xml_diff>
--- a/Deliveries/Project Plan.xlsx
+++ b/Deliveries/Project Plan.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Schedule" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Project Plan</t>
   </si>
@@ -40,15 +40,9 @@
     <t>Deadline</t>
   </si>
   <si>
-    <t>Estimated Duration</t>
-  </si>
-  <si>
     <t>Description &amp; Comments</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Schedule</t>
   </si>
   <si>
@@ -100,7 +94,22 @@
     <t>Prepare CYRS</t>
   </si>
   <si>
-    <t>1 Day</t>
+    <t>Complete CYRS</t>
+  </si>
+  <si>
+    <t>Complete HIS</t>
+  </si>
+  <si>
+    <t>Complete SRS</t>
+  </si>
+  <si>
+    <t>Complete project plan and SIQ based on data from CYRS</t>
+  </si>
+  <si>
+    <t>Estimated Duration (Days)</t>
+  </si>
+  <si>
+    <t>Currently working on modifications asked by Eng. Mohamed Ali</t>
   </si>
 </sst>
 </file>
@@ -158,9 +167,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -169,13 +175,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
+  <dxfs count="17">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -215,32 +249,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:G20" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A4:G20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:G10" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A4:G10"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Member Name" dataDxfId="6"/>
-    <tableColumn id="2" name="Task Name" dataDxfId="5"/>
-    <tableColumn id="3" name="Task Type" dataDxfId="4"/>
-    <tableColumn id="4" name="Start Date" dataDxfId="3"/>
-    <tableColumn id="5" name="Deadline" dataDxfId="2"/>
-    <tableColumn id="6" name="Estimated Duration" dataDxfId="1"/>
-    <tableColumn id="7" name="Description &amp; Comments" dataDxfId="0"/>
+    <tableColumn id="1" name="Member Name" dataDxfId="14"/>
+    <tableColumn id="2" name="Task Name" dataDxfId="13"/>
+    <tableColumn id="3" name="Task Type" dataDxfId="12"/>
+    <tableColumn id="4" name="Start Date" dataDxfId="11"/>
+    <tableColumn id="5" name="Deadline" dataDxfId="10"/>
+    <tableColumn id="6" name="Estimated Duration (Days)" dataDxfId="0">
+      <calculatedColumnFormula>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Description &amp; Comments" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:G5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A4:G5"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Milestone"/>
-    <tableColumn id="2" name="Planned Start Date"/>
-    <tableColumn id="3" name="Actual Start Date"/>
-    <tableColumn id="4" name="Planned End Date"/>
-    <tableColumn id="5" name="Actual End Date"/>
-    <tableColumn id="6" name="Description &amp; Comments"/>
-    <tableColumn id="7" name="Column1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:F8" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A4:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Milestone" dataDxfId="8"/>
+    <tableColumn id="2" name="Planned Start Date" dataDxfId="7"/>
+    <tableColumn id="3" name="Actual Start Date" dataDxfId="6"/>
+    <tableColumn id="4" name="Planned End Date" dataDxfId="5"/>
+    <tableColumn id="5" name="Actual End Date" dataDxfId="4"/>
+    <tableColumn id="6" name="Description &amp; Comments" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -509,16 +544,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="23.3984375" customWidth="1"/>
     <col min="3" max="3" width="16.796875" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
     <col min="5" max="5" width="10.59765625" customWidth="1"/>
@@ -528,15 +563,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -546,13 +581,13 @@
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -562,13 +597,13 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -577,244 +612,160 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43853</v>
+      </c>
+      <c r="E5" s="4">
+        <v>43860</v>
+      </c>
+      <c r="F5" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43852</v>
+      </c>
+      <c r="E6" s="4">
+        <v>43858</v>
+      </c>
+      <c r="F6" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4">
+        <v>43852</v>
+      </c>
+      <c r="E7" s="4">
+        <v>43858</v>
+      </c>
+      <c r="F7" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43852</v>
+      </c>
+      <c r="E8" s="4">
+        <v>43858</v>
+      </c>
+      <c r="F8" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4">
+        <v>43852</v>
+      </c>
+      <c r="E9" s="4">
+        <v>43858</v>
+      </c>
+      <c r="F9" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="5">
-        <v>43853</v>
-      </c>
-      <c r="E5" s="5">
-        <v>43854</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="5">
-        <v>43852</v>
-      </c>
-      <c r="E6" s="5">
-        <v>43853</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="5">
-        <v>43852</v>
-      </c>
-      <c r="E7" s="5">
-        <v>43853</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="5">
-        <v>43852</v>
-      </c>
-      <c r="E8" s="5">
-        <v>43853</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="5">
-        <v>43852</v>
-      </c>
-      <c r="E9" s="5">
-        <v>43853</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="5">
-        <v>43852</v>
-      </c>
-      <c r="E10" s="5">
-        <v>43853</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="D10" s="4">
+        <v>43852</v>
+      </c>
+      <c r="E10" s="4">
+        <v>43858</v>
+      </c>
+      <c r="F10" s="3">
+        <f>SUM(Table1[[#This Row],[Deadline]],-Table1[[#This Row],[Start Date]])</f>
+        <v>6</v>
+      </c>
+      <c r="G10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -830,10 +781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -843,13 +794,13 @@
     <col min="3" max="3" width="16.09765625" customWidth="1"/>
     <col min="4" max="4" width="17.19921875" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="22.296875" customWidth="1"/>
+    <col min="6" max="6" width="37.796875" customWidth="1"/>
     <col min="7" max="7" width="9.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -880,26 +831,95 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4">
+        <v>43852</v>
+      </c>
+      <c r="C5" s="4">
+        <v>43852</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43853</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4">
+        <v>43852</v>
+      </c>
+      <c r="C6" s="4">
+        <v>43852</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43853</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4">
+        <v>43852</v>
+      </c>
+      <c r="C7" s="4">
+        <v>43852</v>
+      </c>
+      <c r="D7" s="4">
+        <v>43853</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4">
+        <v>43853</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43852</v>
+      </c>
+      <c r="D8" s="4">
+        <v>43854</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>